<commit_message>
working on storing indexes locally
</commit_message>
<xml_diff>
--- a/_docs/benchmark_qa_3_temp_zero/llm_responses_document_query_bot.xlsx
+++ b/_docs/benchmark_qa_3_temp_zero/llm_responses_document_query_bot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adaniltd-my.sharepoint.com/personal/30078206_adani_com/Documents/Desktop/LEARNING_FOLDER/_Kolkata_2024/1_LLM/3_Text_query_bot/_docs/benchmark_qa_3_temp_zero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_53DDC8CEDB0904D3C2385E8DD480EC4A778B26BD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{567C7D5F-FA69-4C7E-8C9A-428F874BAF15}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_53DDC8CEDB0904D3C2385E8DD480EC4A778B26BD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A03F7F5-11BD-4F93-86A7-713242F2AD6D}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5220" yWindow="5220" windowWidth="7500" windowHeight="6000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mistral_snow" sheetId="1" r:id="rId1"/>
@@ -2377,51 +2377,51 @@
         <v>0.88522512774699702</v>
       </c>
       <c r="E22" s="5">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" ref="E22:P22" si="0">AVERAGE(E2:E21)</f>
         <v>0.6567308983806095</v>
       </c>
       <c r="F22">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>0.4815811764767669</v>
       </c>
       <c r="G22">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>0.5153731904255946</v>
       </c>
       <c r="H22" s="5">
-        <f>AVERAGE(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>0.45988791691153963</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>0.32219336981763502</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(J2:J21)</f>
+        <f t="shared" si="0"/>
         <v>0.34680840379270417</v>
       </c>
       <c r="K22" s="5">
-        <f>AVERAGE(K2:K21)</f>
+        <f t="shared" si="0"/>
         <v>0.54333600622384304</v>
       </c>
       <c r="L22">
-        <f>AVERAGE(L2:L21)</f>
+        <f t="shared" si="0"/>
         <v>0.39817798999505494</v>
       </c>
       <c r="M22">
-        <f>AVERAGE(M2:M21)</f>
+        <f t="shared" si="0"/>
         <v>0.42448328478915948</v>
       </c>
       <c r="N22" s="5">
-        <f>AVERAGE(N2:N21)</f>
+        <f t="shared" si="0"/>
         <v>0.54900700189483875</v>
       </c>
       <c r="O22">
-        <f>AVERAGE(O2:O21)</f>
+        <f t="shared" si="0"/>
         <v>0.40008430807784362</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(P2:P21)</f>
+        <f t="shared" si="0"/>
         <v>0.42697706861247375</v>
       </c>
     </row>
@@ -3495,55 +3495,55 @@
         <v>209</v>
       </c>
       <c r="D22">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" ref="D22:P22" si="0">AVERAGE(D2:D21)</f>
         <v>0.87445607903859024</v>
       </c>
       <c r="E22">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>0.6242202220294325</v>
       </c>
       <c r="F22">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>0.45883301012356359</v>
       </c>
       <c r="G22">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>0.48929813922345983</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>0.39758240843031029</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>0.3171117416147971</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(J2:J21)</f>
+        <f t="shared" si="0"/>
         <v>0.33085386523654731</v>
       </c>
       <c r="K22">
-        <f>AVERAGE(K2:K21)</f>
+        <f t="shared" si="0"/>
         <v>0.52970531716536207</v>
       </c>
       <c r="L22">
-        <f>AVERAGE(L2:L21)</f>
+        <f t="shared" si="0"/>
         <v>0.39025682615989565</v>
       </c>
       <c r="M22">
-        <f>AVERAGE(M2:M21)</f>
+        <f t="shared" si="0"/>
         <v>0.41509964160269286</v>
       </c>
       <c r="N22">
-        <f>AVERAGE(N2:N21)</f>
+        <f t="shared" si="0"/>
         <v>0.52970531716536207</v>
       </c>
       <c r="O22">
-        <f>AVERAGE(O2:O21)</f>
+        <f t="shared" si="0"/>
         <v>0.39025682615989565</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(P2:P21)</f>
+        <f t="shared" si="0"/>
         <v>0.41509964160269286</v>
       </c>
     </row>
@@ -4615,55 +4615,55 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D22">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" ref="D22:P22" si="0">AVERAGE(D2:D21)</f>
         <v>0.85172260126704435</v>
       </c>
       <c r="E22">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>0.53593384717550319</v>
       </c>
       <c r="F22">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>0.37762763914944208</v>
       </c>
       <c r="G22">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>0.4009995245505113</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>0.29383740866758185</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>0.2011226679806799</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(J2:J21)</f>
+        <f t="shared" si="0"/>
         <v>0.20915807290848853</v>
       </c>
       <c r="K22">
-        <f>AVERAGE(K2:K21)</f>
+        <f t="shared" si="0"/>
         <v>0.43784433746612822</v>
       </c>
       <c r="L22">
-        <f>AVERAGE(L2:L21)</f>
+        <f t="shared" si="0"/>
         <v>0.30414722496341395</v>
       </c>
       <c r="M22">
-        <f>AVERAGE(M2:M21)</f>
+        <f t="shared" si="0"/>
         <v>0.32357384026938119</v>
       </c>
       <c r="N22">
-        <f>AVERAGE(N2:N21)</f>
+        <f t="shared" si="0"/>
         <v>0.43471933746612823</v>
       </c>
       <c r="O22">
-        <f>AVERAGE(O2:O21)</f>
+        <f t="shared" si="0"/>
         <v>0.30345278051896951</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(P2:P21)</f>
+        <f t="shared" si="0"/>
         <v>0.32243747663301747</v>
       </c>
     </row>
@@ -5742,7 +5742,7 @@
         <v>0.70013244028471866</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="E22:P22" si="0">AVERAGE(F2:F21)</f>
+        <f t="shared" ref="F22:P22" si="0">AVERAGE(F2:F21)</f>
         <v>0.43898116625950878</v>
       </c>
       <c r="G22">
@@ -10269,8 +10269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10279,6 +10279,11 @@
     <col min="2" max="2" width="30.109375" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>